<commit_message>
Agregar matriz al codigo y comienzo de todo el recorrido
</commit_message>
<xml_diff>
--- a/Inteligencia Artificial/Practica 2 El viajero/Matriz Estados Viajero.xlsx
+++ b/Inteligencia Artificial/Practica 2 El viajero/Matriz Estados Viajero.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Programacion\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITN\Inteligencia Artificial\Practica 2 El Viajero\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -57,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -157,11 +157,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -169,7 +220,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -181,6 +231,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +609,7 @@
   <dimension ref="A2:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,663 +618,1369 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>2</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>3</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>4</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>5</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>6</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <v>7</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>8</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <v>9</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="8">
         <v>10</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="8">
         <v>11</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="8">
         <v>12</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="8">
         <v>13</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="8">
         <v>14</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="8">
         <v>15</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="8">
         <v>16</v>
       </c>
-      <c r="R2" s="9">
+      <c r="R2" s="8">
         <v>17</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="8">
         <v>18</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="8">
         <v>19</v>
       </c>
-      <c r="U2" s="10">
+      <c r="U2" s="9">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="11">
+        <v>0</v>
+      </c>
+      <c r="C3" s="12">
         <v>87</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="2"/>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12">
+        <v>0</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12">
+        <v>0</v>
+      </c>
+      <c r="M3" s="12">
+        <v>0</v>
+      </c>
+      <c r="N3" s="12">
+        <v>0</v>
+      </c>
+      <c r="O3" s="12">
+        <v>0</v>
+      </c>
+      <c r="P3" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>0</v>
+      </c>
+      <c r="R3" s="12">
+        <v>0</v>
+      </c>
+      <c r="S3" s="12">
+        <v>0</v>
+      </c>
+      <c r="T3" s="12">
+        <v>0</v>
+      </c>
+      <c r="U3" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="14">
         <v>87</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
       <c r="D4" s="1">
         <v>92</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="2"/>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="14">
+        <v>0</v>
+      </c>
       <c r="C5" s="1">
         <v>92</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
       <c r="E5" s="1">
         <v>142</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="2"/>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="14">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
       <c r="D6" s="1">
         <v>142</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
       <c r="F6" s="1">
         <v>98</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
       <c r="H6" s="1">
         <v>85</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="2"/>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="14">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
       <c r="E7" s="1">
         <v>98</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
       <c r="G7" s="1">
         <v>86</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="2"/>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="14">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
       <c r="F8" s="1">
         <v>86</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="2"/>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
       <c r="E9" s="1">
         <v>85</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
       <c r="I9" s="1">
         <v>90</v>
       </c>
       <c r="J9" s="1">
         <v>101</v>
       </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
       <c r="M9" s="1">
         <v>211</v>
       </c>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="2"/>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="14">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
       <c r="H10" s="1">
         <v>90</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="2"/>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="B11" s="14">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
       <c r="H11" s="1">
         <v>101</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
       <c r="K11" s="1">
         <v>97</v>
       </c>
       <c r="L11" s="1">
         <v>138</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="2"/>
+      <c r="M11" s="1">
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="B12" s="14">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
       <c r="J12" s="1">
         <v>97</v>
       </c>
-      <c r="K12" s="1"/>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
       <c r="L12" s="1">
         <v>146</v>
       </c>
-      <c r="M12" s="1"/>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
       <c r="N12" s="1">
         <v>80</v>
       </c>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="2"/>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="B13" s="14">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
       <c r="J13" s="1">
         <v>138</v>
       </c>
       <c r="K13" s="1">
         <v>146</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
       <c r="O13" s="1">
         <v>120</v>
       </c>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="2"/>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
       <c r="H14" s="1">
         <v>211</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
       <c r="N14" s="1">
         <v>99</v>
       </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="2"/>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="1">
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="B15" s="14">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
       <c r="K15" s="1">
         <v>80</v>
       </c>
-      <c r="L15" s="1"/>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
       <c r="M15" s="1">
         <v>99</v>
       </c>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1">
+        <v>0</v>
+      </c>
       <c r="S15" s="1">
         <v>140</v>
       </c>
-      <c r="T15" s="1"/>
+      <c r="T15" s="1">
+        <v>0</v>
+      </c>
       <c r="U15" s="2">
         <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
+      <c r="B16" s="14">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
       <c r="L16" s="1">
         <v>120</v>
       </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
       <c r="P16" s="1">
         <v>75</v>
       </c>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="2"/>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
+      <c r="B17" s="14">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
       <c r="O17" s="1">
         <v>75</v>
       </c>
-      <c r="P17" s="1"/>
+      <c r="P17" s="1">
+        <v>0</v>
+      </c>
       <c r="Q17" s="1">
         <v>70</v>
       </c>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="2"/>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="B18" s="14">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
       <c r="P18" s="1">
         <v>70</v>
       </c>
-      <c r="Q18" s="1"/>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
       <c r="R18" s="1">
         <v>111</v>
       </c>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="2"/>
+      <c r="S18" s="1">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
+        <v>0</v>
+      </c>
+      <c r="U18" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="B19" s="14">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1">
+        <v>0</v>
+      </c>
       <c r="Q19" s="1">
         <v>111</v>
       </c>
-      <c r="R19" s="1"/>
+      <c r="R19" s="1">
+        <v>0</v>
+      </c>
       <c r="S19" s="1">
         <v>118</v>
       </c>
-      <c r="T19" s="1"/>
-      <c r="U19" s="2"/>
+      <c r="T19" s="1">
+        <v>0</v>
+      </c>
+      <c r="U19" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="B20" s="14">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
       <c r="N20" s="1">
         <v>140</v>
       </c>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="3"/>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>0</v>
+      </c>
       <c r="R20" s="1">
         <v>118</v>
       </c>
-      <c r="S20" s="1"/>
+      <c r="S20" s="1">
+        <v>0</v>
+      </c>
       <c r="T20" s="1">
         <v>75</v>
       </c>
-      <c r="U20" s="2"/>
+      <c r="U20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="B21" s="14">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
       <c r="S21" s="1">
         <v>75</v>
       </c>
-      <c r="T21" s="1"/>
+      <c r="T21" s="1">
+        <v>0</v>
+      </c>
       <c r="U21" s="2">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>20</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4">
+      <c r="B22" s="15">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0</v>
+      </c>
+      <c r="N22" s="3">
         <v>151</v>
       </c>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4">
+      <c r="O22" s="3">
+        <v>0</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
         <v>71</v>
       </c>
-      <c r="U22" s="5"/>
+      <c r="U22" s="4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>